<commit_message>
adding file reruns on lab computer
</commit_message>
<xml_diff>
--- a/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Trial 10 Permutations/10.18/Forward simulation/trial_10.18.xlsx
+++ b/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Trial 10 Permutations/10.18/Forward simulation/trial_10.18.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikki\Desktop\Research\Network Comparison\trial 10 permutations\10.18\Forward simulation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416C9A20-1269-4BE2-9652-F07AB6C81CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1212" windowWidth="18348" windowHeight="11748" tabRatio="877" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1530" yWindow="1215" windowWidth="18345" windowHeight="11745" tabRatio="877" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="5" r:id="rId1"/>
@@ -120,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -892,8 +886,8 @@
     <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="348" xr:uid="{C4125B18-9720-4C0A-AA17-EE128D51C7DF}"/>
-    <cellStyle name="Normal 3" xfId="277" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Normal 2" xfId="348"/>
+    <cellStyle name="Normal 3" xfId="277"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1229,21 +1223,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8984375" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.8984375" style="1"/>
+    <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1251,7 +1245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1259,7 +1253,7 @@
         <v>0.30643999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1267,7 +1261,7 @@
         <v>0.30643999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1275,22 +1269,22 @@
         <v>0.30643999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1303,21 +1297,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.8984375" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.8984375" style="1"/>
+    <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1325,7 +1319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1333,7 +1327,7 @@
         <v>0.15323000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1341,7 +1335,7 @@
         <v>0.15323000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1349,7 +1343,7 @@
         <v>0.15323000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
   </sheetData>
@@ -1364,23 +1358,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="6.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="24" width="6.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="10.8984375" style="1"/>
+    <col min="2" max="5" width="6.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="24" width="6.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1424,7 +1418,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1478,7 +1472,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1532,7 +1526,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1586,7 +1580,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1611,7 +1605,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1636,7 +1630,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1661,7 +1655,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1686,7 +1680,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1711,7 +1705,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1736,7 +1730,7 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1761,7 +1755,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1786,7 +1780,7 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1811,7 +1805,7 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1836,7 +1830,7 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1861,7 +1855,7 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1898,19 +1892,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.8984375" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1924,7 +1918,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1938,7 +1932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1952,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1978,19 +1972,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.8984375" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2004,7 +1998,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -2018,7 +2012,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -2026,13 +2020,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2058,20 +2052,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.8984375" style="1"/>
+    <col min="2" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2079,7 +2073,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2087,7 +2081,7 @@
         <v>2E-8</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2095,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2103,7 +2097,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2111,7 +2105,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2119,7 +2113,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2127,7 +2121,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -2135,7 +2129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2143,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2151,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2159,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -2167,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -2175,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -2189,7 +2183,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -2197,7 +2191,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2253,19 +2247,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.8984375" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2273,7 +2267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -2281,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -2289,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>